<commit_message>
feat: adding crud to table
</commit_message>
<xml_diff>
--- a/planilha_organizador_financeiro.xlsx
+++ b/planilha_organizador_financeiro.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,11 +485,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>salario</t>
+          <t>bico</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2075</v>
+        <v>1800</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -497,15 +497,23 @@
       <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>&lt;function receita at 0x000002813BFE3A60&gt;</t>
-        </is>
-      </c>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>alexandro</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>bolinho no farol</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>500</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -515,111 +523,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>pastel</t>
+          <t>jogo playstation</t>
         </is>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>80</v>
+        <v>450</v>
       </c>
       <c r="E5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>alexandro</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>salário</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>2075</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>adriana</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>manicure</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>69.7</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>alexandro</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>abacaxi</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>15</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>alexandro</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>bico</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1800</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>alexandro</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>bolinho no farol</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>500</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>